<commit_message>
added analysis of resazurin
</commit_message>
<xml_diff>
--- a/taylor-shellfish-sept2025/data/metadata/taylor-shellfish-sept2025-plates.xlsx
+++ b/taylor-shellfish-sept2025/data/metadata/taylor-shellfish-sept2025-plates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/resazurin-family-screenings/taylor-shellfish-sept2025/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B1AFD5-EC65-454C-BEB3-24F7E01AFA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A811DC-2BEC-1B46-BA9A-8BECD4E972EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{9506B5CE-A628-164C-A7D7-A7FBD8EB9181}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>date</t>
   </si>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC4D201-160D-7744-A296-617284EC138C}">
   <dimension ref="A1:G1729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1106,6 +1106,272 @@
         <v>68</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>20250904</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>89</v>
+      </c>
+      <c r="D40">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>20250904</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>85</v>
+      </c>
+      <c r="D41">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>20250904</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>65</v>
+      </c>
+      <c r="D42">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>20250904</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <v>52</v>
+      </c>
+      <c r="D43">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>20250904</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>70</v>
+      </c>
+      <c r="D44">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>20250904</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>35</v>
+      </c>
+      <c r="D45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>20250904</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>60</v>
+      </c>
+      <c r="D46">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>20250904</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>37</v>
+      </c>
+      <c r="D47">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>20250904</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48">
+        <v>38</v>
+      </c>
+      <c r="D48">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>20250904</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49">
+        <v>42</v>
+      </c>
+      <c r="D49">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>20250904</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>82</v>
+      </c>
+      <c r="D50">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20250904</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51">
+        <v>68</v>
+      </c>
+      <c r="D51">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>20250904</v>
+      </c>
+      <c r="B52" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52">
+        <v>73</v>
+      </c>
+      <c r="D52">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>20250904</v>
+      </c>
+      <c r="B53" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53">
+        <v>72</v>
+      </c>
+      <c r="D53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>20250904</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54">
+        <v>71</v>
+      </c>
+      <c r="D54">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>20250904</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55">
+        <v>69</v>
+      </c>
+      <c r="D55">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>20250904</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <v>39</v>
+      </c>
+      <c r="D56">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>20250904</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>87</v>
+      </c>
+      <c r="D57">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>20250904</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58">
+        <v>93</v>
+      </c>
+      <c r="D58">
+        <v>96</v>
+      </c>
+    </row>
     <row r="1250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1250" s="1"/>
       <c r="B1250" s="1"/>

</xml_diff>